<commit_message>
modify for the judge prompt, and update the test queries for evaluation
</commit_message>
<xml_diff>
--- a/rag_evaluation_results.xlsx
+++ b/rag_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>华人是怎么烹饪虾类的？</t>
+          <t>Can you explain what is yung chow min? the noodle..and the process of making it? from which page?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,22 +473,29 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sry, I don't know</t>
+          <t>Yung Chow Min is a noodle soup dish named after the city of Yung Chow in China, celebrated there for its exceptional taste.  According to the recipe found on **page 30 of *The Chinese Cook Book***, the procedure is as follows:
+1. Boil 2 lb of fresh noodles in plenty of water until they float (they are then just cooked).
+2. Immediately lift them out and plunge them into a basin of cold water to halt further cooking.
+3. Fish the noodles out again and briefly deep-fry them in hot oil until they become firm and crisp on the outside (this is the distinctive “two-stage” texture).
+4. Return the fried noodles to a pot with 7 cups of “primary soup” (rich chicken stock) and simmer just long enough for them to become soft and absorb flavour.
+5. Separately, make a chicken gravy: combine 1 cup diced cooked chicken, 1½ cups sliced Chinese mushrooms and 1½ cups sliced Chinese water-chestnuts; bind this with a little Chinese gravy (starch-thickened seasoned stock) and heat through.
+6. Pour the hot chicken-mushroom gravy into the noodle soup, stir once, remove from the heat and serve pipping hot.
+These steps create the signature Yung Chow Min: springy noodles inside a fragrant, clear soup topped with savoury chicken, mushroom and water-chestnut gravy—taken directly from page 30 of the cookbook.</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The answer is a canned response indicating a lack of knowledge, providing no useful information.</t>
+          <t>This answer is the best because it provides a more detailed and descriptive explanation of the Yung Chow Min recipe, including specific quantities and clarifying details like the "two-stage" texture. It also explicitly mentions the source as page 30 of *The Chinese Cook Book*, which is more precise.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>华人是怎么烹饪虾类的？</t>
+          <t>Can you explain what is yung chow min? the noodle..and the process of making it? from which page?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -498,22 +505,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sry, I don't know.</t>
+          <t>Yung Chow Min is a noodle dish, where "Min" means noodle and "Yung Chow" is the name of the place in China where this dish is prepared in the most delicious way.
+The process of making Yung Chow Min is as follows:
+(a) Put 2 pounds of noodles into boiling water, and boil until they float on the surface.
+(b) Take out and quickly place them in cold water.
+(c) Put the noodles into boiling oil until they become hard.
+(d) Cook the noodles in 7 cups of primary soup until soft.
+(e) Make a chicken gravy using 1 cup of chicken fragments, 1½ cups Chinese mushrooms, and 1½ cups Chinese water chestnuts. Add this to Chinese gravy.
+(f) Pour the gravy into the soup and stir well. Remove from the stove at once and serve hot.
+This information is from page 30.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The answer is a canned response indicating a lack of knowledge, providing no useful information.</t>
+          <t>This answer provides a good summary of the recipe and correctly identifies the page number. However, it lacks the detail and clarity of the Moonshot answer, making it slightly less helpful.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>华人是怎么烹饪虾类的？</t>
+          <t>Can you explain what is yung chow min? the noodle..and the process of making it? from which page?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -523,24 +538,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>根据背景信息，华人烹饪虾类的方式包括：
-*   **蒸**：例如“金色池塘虾”（SHRIMP IN GOLDEN POND / HAR JING DON），做法是将虾肉铺在混合好的鸡蛋液上蒸20分钟。另一种是“清蒸虾”（STEADIED SHRIMP / DON HAE），这种做法是先将虾油炸5分钟，沥干液体后与竹笋一起放入碗中，加入高汤蒸2小时。
-*   **炒**：例如“炒虾”（Fried Shrimp）和“虾肉杂碎”（Shrimp Chop Suey）。</t>
+          <t>Yung Chow Min is a noodle dish, where "Min" means noodle and "Yung Chow" is a place in China famous for preparing this dish in a delicious way.
+The process of making Yung Chow Min is as follows:
+(a) Put 2 pounds of noodles into boiling water and boil until they float on the surface.
+(b) Take out the noodles and quickly place them in cold water.
+(c) Put the noodles into boiling oil until they become hard.
+(d) Cook the noodles in 7 cups of primary soup until they are soft.
+(e) Make a chicken gravy using 1 cup of chicken fragments, 1.5 cups of Chinese mushrooms, and 1.5 cups of Chinese water chestnuts. Add this to Chinese gravy.
+(f) Pour the prepared gravy into the soup, stir it well, remove from the stove at once, and serve hot.
+This information is from page 30.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>This answer provides specific examples of how Chinese people cook shrimp, including steaming and frying, and even mentions specific dishes. It is the only answer that provides relevant information.</t>
+          <t>This answer is very similar to the Gemini_HuggingFaceEmbeddings answer in content and quality, but since the other Gemini answer is already second best, this one gets 0 points.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What are the main ingredients for cooking chinese-style Chicken?</t>
+          <t>处理食材通常有什么规矩还有禁忌？</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -550,39 +571,35 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>According to the Chinese Cook Book excerpt, common Chinese-style chicken dishes use these primary ingredients:
-- Chicken (usually cut into pieces or fragments)
-- Vegetables:  
-  • Mushrooms  
-  • Water chestnuts (for chop suey)  
-  • Bamboo shoots (for chop suey)  
-  • Celery (for chop suey)  
-  • Ginger root  
-  • Onion  
-  • Spring onion (also called Chinese onion)
-- Sauces/condiments:  
-  • Soy sauce (implied by "Chinese sauce")  
-  • Cornstarch  
-  • Oil  
-  • Salt  
-  • Spicery salt (a fried mixture of spicery powder and salt)
-- Optional flavorings:  
-  • Red dates (for steamed chicken)</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
+          <t>根据所给背景资料，关于中国传统烹饪处理食材的“规矩”主要有以下几条，而“禁忌”部分则未在原文中提及，故具体禁忌尚未列出。  
+规矩（必须遵循的工艺标准）：  
+1. 结构与比例  
+   - 任何一道菜都应由三部分组成：主要肉类、次级蔬菜（如菱角、竹笋、芹菜、香菇等应季蔬菜），以及表面装饰（火腿、鸡肉或叉烧的小丁或约一英寸长的小棒，点缀部分香菜）。  
+   - 遵循“孔子卫生法”：肉量约占蔬菜总量的三分之一。  
+2. 刀工与形态  
+   - 肉块必须与蔬菜块大小、形状相同，且整块保持一致；可视蔬菜尺寸切成丁、条或碎粒，但务必均匀整齐。  
+3. 调味配料  
+   - 装饰物不仅提升外观，也必须兼顾风味，因此香菜（芫荽）用量需足以“助味”而非仅供点缀。  
+4. 基本烹调法  
+   - 传统手段以蒸、炒、煮三大类为核心。  
+关于禁忌，原文未提及任何明确“不能”的事项，因此目前无法给出确定的禁忌内容。</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>This answer is the most comprehensive and detailed, listing a wide range of ingredients commonly used in Chinese-style chicken dishes, including specific vegetables, sauces, and optional flavorings. It provides a clear and well-organized list.</t>
+          <t>Evaluation failed: Expecting value: line 5 column 1 (char 1086)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What are the main ingredients for cooking chinese-style Chicken?</t>
+          <t>处理食材通常有什么规矩还有禁忌？</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -592,224 +609,542 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Based on the provided information, the main ingredients for cooking Chinese-style Chicken dishes commonly include:
-*   Chicken
-*   Mushrooms
-*   Oil
-*   Sauce (or Chinese sauce)
-*   Salt</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
+          <t>根据背景信息，处理食材的规矩主要有以下几点：
+1.  **比例规矩：** 根据孔子的卫生法，肉的用量大约是配菜（次要蔬菜）的三分之一。
+2.  **形状和大小规矩：** 肉应该和蔬菜的大小、形状相同，并且必须均匀。肉可以切成丁、条或碎块，在蔬菜大小有限时，需要根据实际情况判断如何切割。
+背景信息中没有提及具体的食材处理禁忌。</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>This answer is good and provides some of the key ingredients, but it's less detailed than the Moonshot/Kimi answer. It lacks the specificity of vegetables and optional flavorings.</t>
+          <t>Evaluation failed: Expecting value: line 5 column 1 (char 1086)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>处理食材通常有什么规矩还有禁忌？</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gemini_GeminiEmbeddings</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>根据提供的背景信息，处理食材的规矩主要有以下几点：
+1.  **肉与蔬菜的比例**：根据孔子的卫生法则，肉的用量大约是次要蔬菜的三分之一。
+2.  **肉的形状与大小**：肉应该与蔬菜的大小和形状相同，并且必须均匀一致。可以切成丁、条状或碎片，具体根据蔬菜的大小来判断。
+3.  **蒸制方法**：
+    *   蒸制时务必沥干水分或其他液体物质，加入足够的主汤（primary soup）以覆盖食材。
+    *   蒸到刚变软即可，因为在这种状态下食物味道最佳。
+    *   食用前，倒掉主汤，撇去表面的所有油，然后再次放入蒸锅中片刻。
+    *   蒸制时需用旺火。
+4.  **煮制方法**：煮制时，火力只需足够热，以保持食物在沸点即可。
+5.  **炒制方法**：
+    *   炒制时需用旺火。
+    *   食物应不断用炒铲翻动，以确保每个部分都能受热均匀。
+6.  **调味**：根据口味加盐。
+背景信息中没有明确提到处理食材的禁忌。</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Evaluation failed: Expecting value: line 5 column 1 (char 1086)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>中式烹饪是怎么处理鱼类的？有什么讲究。</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Moonshot/Kimi_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>在中式烹饪里，处理鱼类（尤其以你给食谱里的淡水鱼“pike——白梭吻鲈”为例）讲究三个核心环节——去净、剁细、顺搅。具体做法如下：
+1. 去净  
+   ‑ 片掉整张鱼皮，彻底挑净骨刺，只保留净肉，目的是口感细腻、无渣。  
+2. 剁细  
+   ‑ 将鱼肉放进研磨器连打三遍，直到成为极细的糜状；这样做出的丸子弹牙、浮汤不浑。  
+3. 顺搅  
+   ‑ 把鱼糜放入大碗，加入淀粉、盐及少许清水，选好一个方向（比如顺时针）持续搅拌一小时。时间可让盐和淀粉充分抓入肉里，顺向搅拌能让蛋白质充分出胶，丸子弹韧不散。  
+此外，辅以坚果粒、火腿丁和时令蔬菜小粒，可带来香、脆、鲜的多重口感；最后或蒸、或油炸至金黄，都是鱼料理的传统讲究。</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>This answer provides a specific method for preparing fish, focusing on deboning, mincing, and stirring. It's detailed and practical, offering a clear process. However, it's somewhat narrow in scope, focusing on a particular preparation style rather than a broader overview of Chinese fish cooking techniques.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>中式烹饪是怎么处理鱼类的？有什么讲究。</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gemini_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sry, I don't know.</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>This answer is simply an 'I don't know' response, making it irrelevant and unhelpful.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>中式烹饪是怎么处理鱼类的？有什么讲究。</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Gemini_GeminiEmbeddings</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>根据提供的背景信息，中式烹饪对鱼类的处理方式和讲究主要体现在以下几个方面：
+1.  **鱼类选择和处理：**
+    *   会根据菜品选择不同类型的鱼，例如派克鱼（pike）、鳕鱼（cod）或任何淡水鱼。
+    *   **清洁**：所有鱼类烹饪前都需要进行清洁。
+    *   **切割方式多样**：
+        *   有的菜品（如“Hot Water Fish”）要求鱼保持**完整不切割**。
+        *   有的菜品（如“Fish Chop Suey”）则需要将鱼**去骨去皮，切成薄片**（如1/16英寸厚）。
+        *   “Fried Fish”则没有明确切割要求，但通常会是整条或大块。
+2.  **前期准备与调味：**
+    *   **盐腌**：常见做法是在鱼身内外涂抹盐进行腌制（如“Fried Fish”）。
+    *   **热水处理**：例如“Hot Water Fish”会先将整条鳕鱼放入相当于其重量5倍的沸水中加盐浸泡，直到水变温。
+3.  **烹饪方法：**
+    *   **油炸**：将鱼在沸油中炸至金黄（如“Fried Fish”）。
+    *   **炖煮/烩**：油炸后的鱼会加入足够的水、醋和玉米淀粉一起炖煮（如“Fried Fish”）。其他菜品也会在烹饪其他配料后加水一起煮（如“Fish Chop Suey”）。
+    *   **温水浸泡**：独特的“Hot Water Fish”做法，利用高温水和盐对整鱼进行温和处理。
+    *   **配料混合**：鱼可以与其他蔬菜（如蘑菇、姜、竹笋、豆芽）一起炒煮（如“Fish Chop Suey”），鱼肉通常在最后加入并混合。
+4.  **调味与增稠：**
+    *   **中式芡汁（gravy）**：许多鱼类菜品都会在烹饪结束时加入中式芡汁，以增加风味和口感。
+    *   **醋和玉米淀粉**：常用于调味和勾芡，使汤汁浓稠（如“Fried Fish”、“Hot Water Fish”的芡汁中都用到）。
+    *   **其他调味料**：还会用到糖（如“Hot Water Fish”的芡汁）、中式杂烩酱（Chinese Chow Chow，如“Hot Water Fish”）。
+5.  **摆盘与上桌：**
+    *   常用欧芹（parsley）进行装饰，并趁热食用。
+综上所述，中式烹饪在处理鱼类时，非常注重根据菜肴特点选择合适的鱼种、精细的切割与前期处理（去骨、去皮、盐腌或热水浸泡），并结合油炸、炖煮、温水处理等多种烹饪手法，最终通过芡汁的运用达到色香味俱全的效果。</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>This answer gives a comprehensive overview of how fish is handled in Chinese cooking, covering selection, preparation, cooking methods, seasoning, and presentation. It's well-organized and informative, providing a broad understanding of the topic. It is equally good as the first answer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>What are the main ingredients for cooking chinese-style Chicken?</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Moonshot/Kimi_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Looking at the classic Chinese recipes provided, the **main ingredients** commonly used for Chinese-style chicken are:
+1. **Chicken** – typically cut into pieces or fragments  
+2. **Oil** – for stir-frying or frying  
+3. **Salt** – for seasoning  
+4. **Cornstarch** – for texture and coating  
+5. **Sauce (soy sauce implied)** – for flavoring  
+Additionally, **mushrooms** appear frequently (used in Chop Suey and Steamed Chicken), while **ginger root**, **Chinese onion**, and **red dates** are used in more traditional preparations like *Steamed Chicken* (*Ging Guy*).</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>This answer is the most accurate and comprehensive. It lists the core ingredients (chicken, oil, salt, cornstarch, sauce) and then adds context about other common ingredients like mushrooms, ginger, and onion. It also specifies the form of chicken used.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>What are the main ingredients for cooking chinese-style Chicken?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gemini_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Based on the provided recipes for Chinese-style chicken dishes, the main ingredients include:
+*   **Chicken** (whole, cut into fragments, or pieces)
+*   **Oil** (for frying)
+*   **Mushrooms**
+*   **Sauce** (Chinese sauce)
+*   **Salt**
+Other ingredients that appear in specific dishes include water chestnuts, bamboo shoots, celery, ginger root, red dates, Chinese onion, cornstarch, and spicery powder.</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>This answer is also good and lists most of the main ingredients. However, it's slightly less detailed than Moonshot/Kimi_HuggingFaceEmbeddings, missing cornstarch and not explicitly stating soy sauce.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>What are the main ingredients for cooking chinese-style Chicken?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Gemini_GeminiEmbeddings</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>The main ingredients for cooking Chinese-style Chicken, based on the provided information, are:
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Based on the provided background information, the main ingredients for cooking Chinese-style Chicken include:
 *   Chicken
-*   Oil
 *   Primary soup
 *   Chinese gravy
-*   Vegetables (or secondary vegetables)</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+*   Vegetables (or secondary vegetables)
+*   Oil (for frying)
+*   Water (for boiling)
+*   Fried walnuts (for garnish)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>This answer is the least accurate. 'Primary soup' and 'Chinese gravy' are not standard main ingredients in the same way that chicken, oil, and vegetables are. It's also vague compared to the other answers.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>This answer includes less relevant ingredients like 'primary soup' and 'Chinese gravy,' which are not fundamental ingredients but rather components of specific dishes. It also mentions 'fried walnuts for garnish,' which is not a main ingredient. The answer is less accurate and less focused on the core ingredients.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
         <is>
           <t>牛肉适合拿来做什么料理/菜谱？通常都搭配什么食材？</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Moonshot/Kimi_HuggingFaceEmbeddings</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>牛肉适合的料理 / 菜谱  
-• Beef Chop Suey（牛肉杂碎）  
-• Green Pepper Beef（青椒牛肉）  
-——以上两者都出现在文档的“Beef”章节里。
-通常搭配的食材  
-按照「中国烹饪通则」的规定，一道完整的中式牛肉菜应包含三部分：  
-1. 牛肉 – 约只占总量三分之一；应切成与配菜同样的大小与形状，且均匀。  
-2. 辅助蔬菜 – 约占总量三分之二，常用的有：菱角、竹笋、芹菜、香菇等，也可根据时令加入其他蔬菜。  
-3. 顶饰（garnish） – 少量切成丁或条的熟火腿、鸡肉或叉烧，再加一点香菜提味兼装饰。
-这样既能保持卫生比例，又兼顾口感与营养均衡。</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>根据现有资料，牛肉适用的主要料理及常见搭配如下：
+**主要牛肉菜谱 / 菜式：**
+1. **牛肉炒杂碎**（Beef Chop Suey）  
+   属于经典“杂碎”类菜品，和猪肉、鱼版本并列介绍，足见其地位。
+2. **青椒牛肉**（Green Pepper Beef）  
+   注明以青椒（green pepper）为主角，色泽、口感对比鲜明。
+**官方搭配准则（根据《中国烹饪通则》）：**  
+– 任何一道菜都遵循 **“约1/3肉量”** 的原则。  
+– **主料统一大小形状**，配合斩成小丁或1英寸细条的 **火腿、鸡丁、烤猪肉** 作“次级蔬菜”（如荸荠、竹笋、香芹、香菇等时令配菜）共同炒制。  
+– 最终还会以少量 **火腿、鸡肉、烤猪肉丁 + 香芹碎** 作为顶饰，既点香又配色。
+简言之：用牛肉做「牛肉炒杂碎」或「青椒牛肉」最常见。炒制时牛肉与青椒、香芹、适量火腿/鸡丁或烤猪肉条大小一致，保持1/3肉∶2/3蔬菜的比例即可。</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>0.5</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>This answer provides a good overview of dishes and ingredients, and it correctly references the source document's structure (Beef chapter). The inclusion of the 'Chinese Culinary Principles' adds depth, although it might be a bit too general.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>This answer provides a good overview of suitable beef dishes and common pairings, referencing specific dishes and general principles. It's well-structured and informative, but could benefit from more specific ingredient examples.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>牛肉适合拿来做什么料理/菜谱？通常都搭配什么食材？</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Gemini_HuggingFaceEmbeddings</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>根据提供的背景信息，牛肉可以用来制作 'Beef Chop Suey'（牛肉炒杂碎）和 'Green Pepper Beef'（青椒牛肉）。
-通常来说，在中式烹饪中，肉类（包括牛肉）会搭配以下食材：
-*   **次要蔬菜（secondary vegetables）**: 例如荸荠（Chinese water chestnut）、竹笋（bamboo shoot）、芹菜（celery）、香菇（Chinese mushroom），以及其他根据季节选择的蔬菜。
-*   **作为点缀的配料（garnish）**: 例如中式火腿（Chinese ham）、鸡肉（chicken）或烤猪肉（roast pork），这些通常切成小丁或约一英寸长的小条；还会搭配足够的欧芹（parsley）来增味和装饰。
-根据孔子的卫生法则，肉的用量大约是次要蔬菜的三分之一。肉的形状和大小应与蔬菜相同，并保持一致。</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>根据您提供的背景信息，牛肉适合制作的料理或菜谱有：
+*   **Beef Chop Suey**
+*   **Green Pepper Beef**
+通常搭配的食材，根据中式烹饪的通用法则，肉类（包括牛肉）会与以下食材搭配：
+*   **主要蔬菜**：如中华荸荠（Chinese water chestnut）、竹笋（bamboo shoot）、芹菜（celery）、中式蘑菇（Chinese mushroom），以及其他季节性蔬菜。
+*   **点缀/配料**：包括中式火腿（Chinese ham）、鸡肉（chicken）或烤猪肉（roast pork），通常切成小丁或小条，以及香菜（parsley）来增添风味和装饰。
+此外，牛肉的用量通常是次要蔬菜的三分之一左右。</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>0.5</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>This answer is similar in quality to Moonshot. It correctly identifies the dishes and provides a good list of ingredients, including garnish. The reference to Confucius's hygiene rules is a bit odd but comes from the document.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>This answer is similar in quality to Moonshot's answer. It lists the same dishes and provides a decent list of ingredients. The structure is clear and easy to understand.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>牛肉适合拿来做什么料理/菜谱？通常都搭配什么食材？</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Gemini_GeminiEmbeddings</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>根据提供的资料，牛肉适合做以下料理/菜谱：
-1.  **牛肉炒杂碎 (Beef Chop Suey)**
-    通常搭配的食材有：西芹、豆芽、玉米淀粉、汾酒、芝麻油、姜丝、盐、中式酱料、水、中式肉汁。
-2.  **青椒牛肉 (Green Pepper Beef)**
-    通常搭配的食材有：青椒、西芹、豆芽、玉米淀粉、汾酒、芝麻油、姜丝、中式酱料、水、中式肉汁。</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>根据您提供的背景信息，牛肉适合用来制作以下料理/菜谱：
+*   **Beef Chop Suey (牛肉炒杂碎)**
+    *   **主要搭配食材：** 芹菜、豆芽。
+    *   **其他配料：** 玉米淀粉、汾酒、麻油、姜丝、盐、中式酱料。
+*   **Green Pepper Beef (青椒牛肉)**
+    *   **主要搭配食材：** 青椒、芹菜、豆芽。
+    *   **其他配料：** 玉米淀粉、汾酒、麻油、姜丝、中式酱料。
+总的来说，牛肉在这些菜谱中常与芹菜、豆芽、青椒等蔬菜搭配，并使用玉米淀粉、汾酒、麻油、姜丝和中式酱料进行调味。</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>This answer is the most comprehensive and specific. It not only lists the dishes but also provides detailed ingredient lists for each, including both main ingredients and seasonings. This level of detail makes it the most helpful and informative response.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>How to make steamed buns?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Moonshot/Kimi_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sry, I don't know</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>0</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>This answer focuses too narrowly on the specific ingredients for Beef Chop Suey and Green Pepper Beef, neglecting the broader range of possibilities. It's less helpful overall compared to the other two answers.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Can you explain the process of making dumplings?</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>The answer is a canned response indicating a lack of knowledge, making it irrelevant.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>How to make steamed buns?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Gemini_HuggingFaceEmbeddings</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sry, I don't know</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>The answer is a canned response indicating a lack of knowledge, making it irrelevant.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>How to make steamed buns?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Gemini_GeminiEmbeddings</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>To make steamed buns, follow these steps:
+1.  **Dough Preparation:**
+    *   Put the dough into a pan, cover well with a towel, and let it stand overnight.
+    *   In the morning, turn the dough out onto a mixing-board. Knead it and let it stand until it rises to double its size.
+2.  **Forming and Filling (Choose your filling):**
+    *   **For Bean-Filled Buns:**
+        *   Roll the dough biscuits flat.
+        *   Fill each one with beans, wrapping the dough carefully around the beans to make a perfect ball.
+    *   **For Meat and Cheese Filled Buns:**
+        *   Cut the dough into the size of biscuits and roll flat.
+        *   Add chopped roast pork, chopped frankfurter, red cheese, and salt. The amount of meat and cheese should be about one-half that of the dough.
+        *   Wrap the mixture up into a ball, closing it carefully to make a perfect ball.
+3.  **Steaming:**
+    *   Place the formed dough biscuits/balls in a double-boiler for 10 minutes before putting them on the fire/stove.
+    *   Steam for an hour.</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>This answer provides a detailed and relevant recipe for making steamed buns, including dough preparation, filling options, and steaming instructions. It directly addresses the question and offers practical steps.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>What is the cooking time for roasted duck? what ingredients are needed?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Moonshot/Kimi_HuggingFaceEmbeddings</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Sry, I don't know</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>The answer is a canned response indicating a lack of knowledge, making it irrelevant.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Can you explain the process of making dumplings?</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>For the basic Roast Duck (SUE AEP)：
+Cooking time  
+- Roast for 1 hour.
+Ingredients needed  
+- 2 ducks, about 4 lb each  
+- 2 tsp spicery powder  
+- 2 cups Chinese sauce  
+- Few drops of sesame-seed oil  
+- 2 tsp salt</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>The answer provides the cooking time and ingredients needed for roasted duck, directly addressing the question. It's clear and concise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>What is the cooking time for roasted duck? what ingredients are needed?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Gemini_HuggingFaceEmbeddings</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Sry, I don't know.</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>The answer is a canned response indicating a lack of knowledge, making it irrelevant.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Can you explain the process of making dumplings?</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Based on the provided information:
+**Cooking Time for Roasted Duck:**
+Roast for 1 hour.
+**Ingredients Needed for Roasted Duck:**
+*   2 ducks (about 4 pounds each)
+*   2 teaspoonfuls spicery powder
+*   2 cups Chinese sauce
+*   A few drops of sesamum-seed oil
+*   2 teaspoonfuls salt</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>The answer provides the cooking time and ingredients needed for roasted duck, directly addressing the question. It's clear and concise.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>What is the cooking time for roasted duck? what ingredients are needed?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Gemini_GeminiEmbeddings</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Based on the information provided, here's a process for making dough-based items that are filled and steamed, which resembles dumpling making:
-1.  Roll dough flat.
-2.  Fill each piece of dough with your chosen filling (e.g., beans, or meat and cheese, where the filling amount should be about one-half that of the dough).
-3.  Wrap the dough around the filling to make a perfect ball.
-4.  Close the dough carefully.
-5.  Let the dough balls stand in a double-boiler for 10 minutes before putting them on the fire/stove.
-6.  Steam for half an hour.
-Additionally, when working with the dough, it's mentioned to dredge your hands well with flour and use as little flour as possible when kneading, only enough to prevent sticking.</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>This answer provides a reasonable, albeit generic, description of the dumpling-making process. While it lacks specific details (e.g., types of dough, folding techniques), it outlines the core steps of rolling dough, filling it, wrapping, and steaming. It's the only answer that attempts to address the question, making it the best by default.</t>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>For roasted duck, the cooking time is 1 hour.
+The ingredients needed are:
+*   2 ducks (about 4 pounds each)
+*   2 teaspoonfuls spicery powder
+*   2 cups Chinese sauce
+*   A few drops of sesamum-seed oil
+*   2 teaspoonfuls salt</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>The answer provides the cooking time and ingredients needed for roasted duck, directly addressing the question. It's clear and concise. All answers are of similar quality and provide the same information.</t>
         </is>
       </c>
     </row>

</xml_diff>